<commit_message>
Sign In Test PAssed
</commit_message>
<xml_diff>
--- a/src/main/java/com/ebfs/qa/testdata/EBFSTestData.xlsx
+++ b/src/main/java/com/ebfs/qa/testdata/EBFSTestData.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NaveenKhunteta/Documents/MyPOMFramework/PageObjectModel/src/main/java/com/crm/qa/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khaledhasan/Desktop/Java_Github/Frame_Work/EBFS-PageFactory/src/main/java/com/ebfs/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr documentId="13_ncr:1_{632B4535-559C-EC42-84E5-C94AF2403A9E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
+    <workbookView activeTab="3" tabRatio="500" windowHeight="16640" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
   </bookViews>
   <sheets>
-    <sheet name="contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="deals" sheetId="2" r:id="rId2"/>
-    <sheet name="tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="contacts" r:id="rId1" sheetId="1"/>
+    <sheet name="deals" r:id="rId2" sheetId="2"/>
+    <sheet name="tasks" r:id="rId3" sheetId="3"/>
+    <sheet name="SignIn" r:id="rId4" sheetId="4"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
   <si>
     <t>title</t>
   </si>
@@ -77,13 +79,44 @@
   </si>
   <si>
     <t>Ebay</t>
+  </si>
+  <si>
+    <t>Testcase Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>Verify_ebfs_Login</t>
+  </si>
+  <si>
+    <t>shamim@gmail.com</t>
+  </si>
+  <si>
+    <t>shamim123@ebfs</t>
+  </si>
+  <si>
+    <t>khaledhasanb@gmail.com</t>
+  </si>
+  <si>
+    <t>khaled1234567890</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +127,22 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -123,21 +172,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+  <cellXfs count="4">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -148,10 +204,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -186,7 +242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -221,7 +277,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -315,21 +371,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -346,7 +402,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -398,17 +454,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -471,30 +527,91 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07407D6-D963-034C-8A8C-A1FF0A7BDA73}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="200">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="24.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="36.83203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink display="khaledhasanb@gmail.com" r:id="rId1" ref="B2" xr:uid="{C205ED14-5328-654D-89F9-58FB7C7EF4DC}"/>
+    <hyperlink display="mailto:shamim@gmail.com" r:id="rId2" ref="B3" xr:uid="{28C4862D-97F1-BD4A-A55F-FC3E811F7455}"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Product category Test
</commit_message>
<xml_diff>
--- a/src/main/java/com/ebfs/qa/testdata/EBFSTestData.xlsx
+++ b/src/main/java/com/ebfs/qa/testdata/EBFSTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khaledhasan/Desktop/Java_Github/Frame_Work/EBFS-PageFactory/src/main/java/com/ebfs/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{479F06A0-F59F-274A-8558-ABF4732DDCD5}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
+  <xr:revisionPtr documentId="13_ncr:1_{181641DB-16F8-6342-91EB-8C425811A767}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
     <workbookView activeTab="3" tabRatio="500" windowHeight="16640" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>title</t>
   </si>
@@ -560,7 +560,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" zoomScale="200">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,6 +600,9 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Revert "Sign In Test Passed"
</commit_message>
<xml_diff>
--- a/src/main/java/com/ebfs/qa/testdata/EBFSTestData.xlsx
+++ b/src/main/java/com/ebfs/qa/testdata/EBFSTestData.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khaledhasan/Desktop/Java_Github/Frame_Work/EBFS-PageFactory/src/main/java/com/ebfs/qa/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/NaveenKhunteta/Documents/MyPOMFramework/PageObjectModel/src/main/java/com/crm/qa/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{181641DB-16F8-6342-91EB-8C425811A767}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46"/>
   <bookViews>
-    <workbookView activeTab="3" tabRatio="500" windowHeight="16640" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="contacts" r:id="rId1" sheetId="1"/>
-    <sheet name="deals" r:id="rId2" sheetId="2"/>
-    <sheet name="tasks" r:id="rId3" sheetId="3"/>
-    <sheet name="SignIn" r:id="rId4" sheetId="4"/>
+    <sheet name="contacts" sheetId="1" r:id="rId1"/>
+    <sheet name="deals" sheetId="2" r:id="rId2"/>
+    <sheet name="tasks" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>title</t>
   </si>
@@ -79,44 +77,13 @@
   </si>
   <si>
     <t>Ebay</t>
-  </si>
-  <si>
-    <t>Testcase Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>Verify_ebfs_Login</t>
-  </si>
-  <si>
-    <t>shamim@gmail.com</t>
-  </si>
-  <si>
-    <t>shamim123@ebfs</t>
-  </si>
-  <si>
-    <t>khaledhasanb@gmail.com</t>
-  </si>
-  <si>
-    <t>khaled1234567890</t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -127,22 +94,6 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -172,28 +123,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -204,10 +148,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -242,7 +186,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -277,7 +221,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -371,21 +315,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -402,7 +346,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -454,17 +398,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -527,94 +471,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07407D6-D963-034C-8A8C-A1FF0A7BDA73}">
-  <dimension ref="A1:E3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="200">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="24.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="36.83203125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink display="khaledhasanb@gmail.com" r:id="rId1" ref="B2" xr:uid="{C205ED14-5328-654D-89F9-58FB7C7EF4DC}"/>
-    <hyperlink display="mailto:shamim@gmail.com" r:id="rId2" ref="B3" xr:uid="{28C4862D-97F1-BD4A-A55F-FC3E811F7455}"/>
-  </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>